<commit_message>
adding memory cals for generalised star distance
</commit_message>
<xml_diff>
--- a/dMagMemoryAndProcessTrack.xlsx
+++ b/dMagMemoryAndProcessTrack.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t xml:space="preserve">Computer memory is defined with respect to C conventions, Python conventions may blow these up</t>
   </si>
@@ -242,14 +242,21 @@
   </si>
   <si>
     <t xml:space="preserve">If I known dMagLim as a function of time, I should be able to reformat v1,v2 as functions of time Over a limited range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To make this broadly applicable to many stars, we will need to encode the delta d of these v3,v4,v5,v6 limits. That is, the distance classification for which the solution space changes (i.e. v1,v2 added or subtracted) or v3,v4 cease to exist, or v5,v6 cease to exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For this, it may be benificial to break down stars by binned groupings. For close stars, make the calculations unique, but for further stars, bin the IWA and OWA calculations. i.e. closes 10 stars each have their own bins, then divide 100 bins among the remaining out to 30pc. Lets say this could all be done with less than 100 different bins, this means (possibly) 100*4*8*10^8 v3 v4 v5 v6 edges to calculate…. Too much memory. Lets assume we can reduce this by 1 order of magnitude with our bit array indicating where we don’t need to calculate… that is acceptable but the bit savings must be good!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -315,7 +322,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,6 +333,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -345,10 +356,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK45"/>
+  <dimension ref="A1:AK49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1368,22 +1379,54 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
+      <c r="E39" s="0" t="n">
+        <f aca="false">E38+D39</f>
+        <v>17900000072</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">$E$2-E39</f>
+        <v>246099999928</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
+      <c r="E40" s="0" t="n">
+        <f aca="false">E39+D40</f>
+        <v>17900000072</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">$E$2-E40</f>
+        <v>246099999928</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
+      <c r="E41" s="0" t="n">
+        <f aca="false">E40+D41</f>
+        <v>17900000072</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">$E$2-E41</f>
+        <v>246099999928</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C42" s="2"/>
-    </row>
-    <row r="43" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="0" t="n">
+        <f aca="false">E41+D42</f>
+        <v>17900000072</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <f aca="false">$E$2-E42</f>
+        <v>246099999928</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
         <v>71</v>
       </c>
@@ -1391,15 +1434,95 @@
         <f aca="false">8*10^8</f>
         <v>800000000</v>
       </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">E42+D43</f>
+        <v>18700000072</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <f aca="false">$E$2-E43</f>
+        <v>245299999928</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="E44" s="0" t="n">
+        <f aca="false">E43+D44</f>
+        <v>18700000072</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">$E$2-E44</f>
+        <v>245299999928</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">E44+D45</f>
+        <v>18700000072</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">$E$2-E45</f>
+        <v>245299999928</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="2"/>
+      <c r="E46" s="0" t="n">
+        <f aca="false">E45+D46</f>
+        <v>18700000072</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">$E$2-E46</f>
+        <v>245299999928</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">E46+D47</f>
+        <v>18700000072</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <f aca="false">$E$2-E47</f>
+        <v>245299999928</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3"/>
+      <c r="B48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">100*8*4*10^8</f>
+        <v>320000000000</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">E47+D48</f>
+        <v>338700000072</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <f aca="false">$E$2-E48</f>
+        <v>-74700000072</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="0" t="n">
+        <f aca="false">10*8*4*10^8</f>
+        <v>32000000000</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">E47+D49</f>
+        <v>50700000072</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <f aca="false">$E$2-E49</f>
+        <v>213299999928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more testing on equations for finding maxS
</commit_message>
<xml_diff>
--- a/dMagMemoryAndProcessTrack.xlsx
+++ b/dMagMemoryAndProcessTrack.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="143">
   <si>
     <t xml:space="preserve">nplan</t>
   </si>
@@ -275,6 +276,180 @@
   </si>
   <si>
     <t xml:space="preserve">Calculate (dt_enter1*0.5+dt_enter2*0.5) to get average time until the planet enters FoV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coeff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rows of Eqn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">term in row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^2y^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xy^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^2y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^3y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xy^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grouping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^2y^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^3y^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x^3y^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has negative?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90-180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180-270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">270-360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why make the plus minus table above? Because now I will know which terms are positive and which terms are negative.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we know all the term constants (see table above), we can know which of the terms are negative and positive so we may set them appropriately equal to one another</t>
   </si>
 </sst>
 </file>
@@ -289,6 +464,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,7 +529,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:AK58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -393,13 +569,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="2.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="2.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="5.28"/>
@@ -407,10 +583,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="2.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="32" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="3.51"/>
@@ -1717,4 +1893,716 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA9" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <f aca="false">SUM(D10:AA10)</f>
+        <v>30</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA13" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA15" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K16" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K18" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding descriptor for function
</commit_message>
<xml_diff>
--- a/dMagMemoryAndProcessTrack.xlsx
+++ b/dMagMemoryAndProcessTrack.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="144">
   <si>
     <t xml:space="preserve">nplan</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t xml:space="preserve">Calculate (dt_enter1*0.5+dt_enter2*0.5) to get average time until the planet enters FoV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsbydnu</t>
   </si>
   <si>
     <t xml:space="preserve">term</t>
@@ -1902,8 +1905,8 @@
   </sheetPr>
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1912,22 +1915,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -1956,82 +1962,82 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,76 +2045,76 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,76 +2122,76 @@
         <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,114 +2199,114 @@
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="N6" s="0" t="s">
         <v>26</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K9" s="0" t="s">
+      <c r="M9" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="N9" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="P9" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
@@ -2365,235 +2371,235 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA14" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K16" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K17" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K18" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>